<commit_message>
refactor : enhance file parsing logic to support all Java and SQL date/time types
</commit_message>
<xml_diff>
--- a/entity-instantiator-spring/src/test/resources/file-source/file_source.xlsx
+++ b/entity-instantiator-spring/src/test/resources/file-source/file_source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wonjae/Java/EntityInstantiator/entity-instantiator-spring/src/test/resources/file-source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C39CE75-9A5B-F242-AE30-B70FB4E05CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243ED6C2-446D-2A4A-B6EE-BF069D8FBADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{0BBCF34A-D82F-9046-B92F-440159AE1606}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>name</t>
   </si>
@@ -44,79 +44,19 @@
     <t>email</t>
   </si>
   <si>
-    <t>balance</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>localDate</t>
-  </si>
-  <si>
-    <t>localTime</t>
-  </si>
-  <si>
-    <t>localDateTime</t>
-  </si>
-  <si>
-    <t>offsetDateTime</t>
-  </si>
-  <si>
-    <t>offsetTime</t>
-  </si>
-  <si>
-    <t>instant</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>calendar</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>sqlDate</t>
-  </si>
-  <si>
-    <t>timestamp</t>
-  </si>
-  <si>
-    <t>byteArray</t>
-  </si>
-  <si>
-    <t>charArray</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>wonjae</t>
   </si>
   <si>
     <t>wonjae@example.com</t>
   </si>
   <si>
-    <t>2025-10-08T13:45:30</t>
-  </si>
-  <si>
-    <t>2025-10-08T13:45:30+09:00</t>
-  </si>
-  <si>
-    <t>13:45:30+09:00</t>
-  </si>
-  <si>
-    <t>2025-10-08T04:45:30Z</t>
-  </si>
-  <si>
-    <t>aGVsbG8=</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>ADMIN</t>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>qwer</t>
   </si>
 </sst>
 </file>
@@ -511,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F0E6E4-C55C-4B40-9ED6-02C6D23467B0}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,113 +474,69 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>1.23456789012345E+19</v>
-      </c>
-      <c r="D2">
-        <v>12345.67</v>
-      </c>
-      <c r="E2" s="3">
-        <v>45938</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0.57326388888888891</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="3">
-        <v>45938</v>
-      </c>
-      <c r="L2" s="3">
-        <v>45938</v>
-      </c>
-      <c r="M2" s="4">
-        <v>0.57326388888888891</v>
-      </c>
-      <c r="N2" s="3">
-        <v>45938</v>
-      </c>
-      <c r="O2" s="5">
-        <v>45938.573263888888</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" t="s">
-        <v>26</v>
+        <v>3</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="mailto:wonjae@example.com" xr:uid="{73FDECBE-E2BE-944E-873A-19C48FE0F919}"/>
+    <hyperlink ref="B4" r:id="rId1" display="mailto:wonjae@example.com" xr:uid="{55B03342-303A-3949-85BC-4205BD4AE986}"/>
+    <hyperlink ref="B3" r:id="rId2" display="mailto:wonjae@example.com" xr:uid="{84BA29C8-62E6-CE43-AE42-8CD1E2F1EE23}"/>
+    <hyperlink ref="B2" r:id="rId3" display="mailto:wonjae@example.com" xr:uid="{73FDECBE-E2BE-944E-873A-19C48FE0F919}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>